<commit_message>
Added scripts to run from command line. Redone logic of some methods. Made xlsx files blank.
</commit_message>
<xml_diff>
--- a/Test_file_1.xlsx
+++ b/Test_file_1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ECF8D2-26D6-4AC6-B0A5-1BE310DA0595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102C65D5-23EC-48A3-9940-B3C39F57D4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Оценка компетенций" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>ФИО (заполнить самостоятельно)</t>
   </si>
@@ -90,18 +90,6 @@
   </si>
   <si>
     <t>Баллы от 1 до 5</t>
-  </si>
-  <si>
-    <t>Из Scala и Python выбираем одну компетенцию для ДИ и оцениваем её (инженер + PO). Знание второго языка должно быть не более, чем на 2 уровня ниже</t>
-  </si>
-  <si>
-    <t>Из Airflow и Oozie на аттестацию идёт на выбор одна из тем, которая используется в текущем проекте</t>
-  </si>
-  <si>
-    <t>Опционально, если есть на проекте</t>
-  </si>
-  <si>
-    <t>Запрашивает Даша у РО</t>
   </si>
   <si>
     <t>1.111</t>
@@ -348,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -416,9 +404,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -487,12 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -777,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K30"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -788,37 +767,37 @@
     <col min="2" max="2" width="16.44140625" style="7" customWidth="1"/>
     <col min="3" max="8" width="34.33203125" style="5" customWidth="1"/>
     <col min="9" max="9" width="26.33203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" style="31" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="31" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" style="30" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" style="30" customWidth="1"/>
     <col min="12" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
@@ -828,17 +807,17 @@
       <c r="C6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="42" t="s">
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="43"/>
+      <c r="J6" s="42"/>
     </row>
     <row r="7" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
@@ -848,27 +827,27 @@
       <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="28" t="s">
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="11">
         <v>1</v>
       </c>
@@ -884,9 +863,9 @@
       <c r="H8" s="11">
         <v>5</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
@@ -897,15 +876,15 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="11">
         <v>1</v>
       </c>
@@ -921,9 +900,9 @@
       <c r="H10" s="11">
         <v>5</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
@@ -936,11 +915,11 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="32"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
@@ -953,11 +932,11 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="39">
+      <c r="I12" s="29"/>
+      <c r="J12" s="38">
         <v>2.12121</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -970,11 +949,11 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="32"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
@@ -987,11 +966,11 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="39">
+      <c r="I14" s="29"/>
+      <c r="J14" s="38">
         <v>4</v>
       </c>
-      <c r="K14" s="32"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
@@ -1004,11 +983,11 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="39">
+      <c r="I15" s="29"/>
+      <c r="J15" s="38">
         <v>5</v>
       </c>
-      <c r="K15" s="32"/>
+      <c r="K15" s="31"/>
     </row>
     <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
@@ -1021,11 +1000,11 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="32"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
@@ -1038,11 +1017,11 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="39">
+      <c r="I17" s="29"/>
+      <c r="J17" s="38">
         <v>7.234</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
@@ -1055,11 +1034,11 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="39">
+      <c r="I18" s="29"/>
+      <c r="J18" s="38">
         <v>8.5500000000000007</v>
       </c>
-      <c r="K18" s="32"/>
+      <c r="K18" s="31"/>
     </row>
     <row r="19" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
@@ -1072,11 +1051,11 @@
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="39">
+      <c r="I19" s="29"/>
+      <c r="J19" s="38">
         <v>9</v>
       </c>
-      <c r="K19" s="32"/>
+      <c r="K19" s="31"/>
     </row>
     <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
@@ -1089,9 +1068,9 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="32"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="31"/>
     </row>
     <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
@@ -1104,11 +1083,11 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="32"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
@@ -1122,10 +1101,10 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="39">
+      <c r="J22" s="38">
         <v>12</v>
       </c>
-      <c r="K22" s="32"/>
+      <c r="K22" s="31"/>
     </row>
     <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
@@ -1139,10 +1118,10 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="39">
+      <c r="J23" s="38">
         <v>13</v>
       </c>
-      <c r="K23" s="32"/>
+      <c r="K23" s="31"/>
     </row>
     <row r="24" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
@@ -1156,8 +1135,8 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="32"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="31"/>
     </row>
     <row r="25" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
@@ -1171,10 +1150,10 @@
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="K25" s="32"/>
+      <c r="J25" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
@@ -1188,10 +1167,10 @@
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="39">
+      <c r="J26" s="38">
         <v>16</v>
       </c>
-      <c r="K26" s="32"/>
+      <c r="K26" s="31"/>
     </row>
     <row r="27" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
@@ -1205,10 +1184,10 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="10"/>
-      <c r="J27" s="34" t="s">
+      <c r="J27" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="32"/>
+      <c r="K27" s="31"/>
     </row>
     <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
@@ -1222,10 +1201,10 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="10"/>
-      <c r="J28" s="34" t="s">
+      <c r="J28" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K28" s="32"/>
+      <c r="K28" s="31"/>
     </row>
     <row r="29" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
@@ -1239,10 +1218,10 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="34" t="s">
+      <c r="J29" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="32"/>
+      <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
@@ -1256,10 +1235,10 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="10"/>
-      <c r="J30" s="34" t="s">
+      <c r="J30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="32"/>
+      <c r="K30" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:H30" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -1323,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1314,7 @@
     <col min="4" max="4" width="46.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1346,7 +1325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>14</v>
       </c>
@@ -1355,7 +1334,7 @@
       </c>
       <c r="C2" s="24"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1343,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>14</v>
       </c>
@@ -1373,7 +1352,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1381,11 +1360,8 @@
         <v>14</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>14</v>
       </c>
@@ -1393,9 +1369,8 @@
         <v>14</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="51"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>14</v>
       </c>
@@ -1403,9 +1378,8 @@
         <v>14</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="51"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>14</v>
       </c>
@@ -1413,9 +1387,8 @@
         <v>14</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="51"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
@@ -1423,9 +1396,8 @@
         <v>14</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="27"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>14</v>
       </c>
@@ -1433,11 +1405,8 @@
         <v>14</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="51" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>14</v>
       </c>
@@ -1445,9 +1414,8 @@
         <v>14</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="51"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
@@ -1455,9 +1423,8 @@
         <v>14</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>14</v>
       </c>
@@ -1465,11 +1432,8 @@
         <v>14</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1442,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
@@ -1487,7 +1451,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1460,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>14</v>
       </c>
@@ -1505,7 +1469,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>14</v>
       </c>
@@ -1514,7 +1478,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>14</v>
       </c>
@@ -1522,11 +1486,8 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
@@ -1534,9 +1495,8 @@
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="52"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>14</v>
       </c>
@@ -1544,9 +1504,8 @@
         <v>14</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="52"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>14</v>
       </c>
@@ -1554,14 +1513,8 @@
         <v>14</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D19:D22"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>